<commit_message>
Gunluk bulten guncelleme - 10.02.2026 12:43
</commit_message>
<xml_diff>
--- a/guncel_json/gunlukmaclar.xlsx
+++ b/guncel_json/gunlukmaclar.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="373">
   <si>
     <t>Id</t>
   </si>
@@ -695,505 +695,442 @@
     <t>IYScore K13</t>
   </si>
   <si>
-    <t>YuBydMGL</t>
-  </si>
-  <si>
-    <t>PORTUGAL Liga Portugal</t>
-  </si>
-  <si>
-    <t>FC Porto</t>
-  </si>
-  <si>
-    <t>Sporting CP</t>
+    <t>Kxy4K6zR</t>
+  </si>
+  <si>
+    <t>ENGLAND Premier League</t>
+  </si>
+  <si>
+    <t>West Ham United</t>
+  </si>
+  <si>
+    <t>Manchester United</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t>3.75</t>
+  </si>
+  <si>
+    <t>4.50</t>
+  </si>
+  <si>
+    <t>3.70</t>
+  </si>
+  <si>
+    <t>4.20</t>
+  </si>
+  <si>
+    <t>1.85</t>
+  </si>
+  <si>
+    <t>1.70</t>
+  </si>
+  <si>
+    <t>hxQwmjyp</t>
+  </si>
+  <si>
+    <t>PORTUGAL Liga Portugal 2</t>
+  </si>
+  <si>
+    <t>Paços de Ferreira</t>
+  </si>
+  <si>
+    <t>Sporting CP B</t>
+  </si>
+  <si>
+    <t>2.75</t>
+  </si>
+  <si>
+    <t>2.88</t>
+  </si>
+  <si>
+    <t>3.00</t>
+  </si>
+  <si>
+    <t>2.38</t>
+  </si>
+  <si>
     <t>2.30</t>
   </si>
   <si>
+    <t>O40yKlB7</t>
+  </si>
+  <si>
+    <t>ENGLAND Championship</t>
+  </si>
+  <si>
+    <t>Birmingham City</t>
+  </si>
+  <si>
+    <t>West Bromwich Albion</t>
+  </si>
+  <si>
+    <t>1.76</t>
+  </si>
+  <si>
+    <t>1.81</t>
+  </si>
+  <si>
+    <t>3.40</t>
+  </si>
+  <si>
+    <t>4.10</t>
+  </si>
+  <si>
+    <t>4.33</t>
+  </si>
+  <si>
+    <t>jHoo92Bk</t>
+  </si>
+  <si>
+    <t>ITALIEN Coppa Italia</t>
+  </si>
+  <si>
+    <t>SSC Neapel</t>
+  </si>
+  <si>
+    <t>Como 1907</t>
+  </si>
+  <si>
+    <t>2.05</t>
+  </si>
+  <si>
+    <t>2.70</t>
+  </si>
+  <si>
     <t>3.20</t>
   </si>
   <si>
+    <t>3.60</t>
+  </si>
+  <si>
+    <t>SrvT2keT</t>
+  </si>
+  <si>
+    <t>SCHOTTLAND Premier League</t>
+  </si>
+  <si>
+    <t>Heart of Midlothian</t>
+  </si>
+  <si>
+    <t>Hibernian FC</t>
+  </si>
+  <si>
+    <t>1.66</t>
+  </si>
+  <si>
+    <t>3.50</t>
+  </si>
+  <si>
+    <t>4.75</t>
+  </si>
+  <si>
+    <t>4.00</t>
+  </si>
+  <si>
+    <t>GIoqfBXb</t>
+  </si>
+  <si>
+    <t>DEUTSCHLAND DFB Pokal</t>
+  </si>
+  <si>
+    <t>Hertha BSC</t>
+  </si>
+  <si>
+    <t>SC Freiburg</t>
+  </si>
+  <si>
+    <t>2.90</t>
+  </si>
+  <si>
+    <t>3.30</t>
+  </si>
+  <si>
+    <t>1.95</t>
+  </si>
+  <si>
+    <t>IRLAYmQ0</t>
+  </si>
+  <si>
+    <t>Leicester City</t>
+  </si>
+  <si>
+    <t>FC Southampton</t>
+  </si>
+  <si>
     <t>3.10</t>
   </si>
   <si>
-    <t>3.00</t>
-  </si>
-  <si>
-    <t>zLZxmsU0</t>
-  </si>
-  <si>
-    <t>PERU Liga 1</t>
-  </si>
-  <si>
-    <t>FC Cajamarca</t>
-  </si>
-  <si>
-    <t>Deportivo Garcilaso</t>
+    <t>2.15</t>
+  </si>
+  <si>
+    <t>2.20</t>
+  </si>
+  <si>
+    <t>EgFJWRfD</t>
+  </si>
+  <si>
+    <t>Oxford United</t>
+  </si>
+  <si>
+    <t>Norwich City</t>
+  </si>
+  <si>
+    <t>2.82</t>
+  </si>
+  <si>
+    <t>2.25</t>
+  </si>
+  <si>
+    <t>zPwvTQAc</t>
+  </si>
+  <si>
+    <t>ENGLAND League One</t>
+  </si>
+  <si>
+    <t>Mansfield Town</t>
+  </si>
+  <si>
+    <t>Peterborough United</t>
+  </si>
+  <si>
+    <t>2.32</t>
+  </si>
+  <si>
+    <t>2.65</t>
+  </si>
+  <si>
+    <t>M3KYH02d</t>
+  </si>
+  <si>
+    <t>Wigan Athletic</t>
+  </si>
+  <si>
+    <t>FC Reading</t>
+  </si>
+  <si>
+    <t>2.45</t>
+  </si>
+  <si>
+    <t>2.40</t>
+  </si>
+  <si>
+    <t>YZmnEk95</t>
+  </si>
+  <si>
+    <t>ENGLAND League Two</t>
+  </si>
+  <si>
+    <t>Crawley</t>
+  </si>
+  <si>
+    <t>Cambridge United</t>
+  </si>
+  <si>
+    <t>2.10</t>
+  </si>
+  <si>
+    <t>vgv18Kxp</t>
+  </si>
+  <si>
+    <t>Shrewsbury Town</t>
+  </si>
+  <si>
+    <t>AFC Barrow</t>
+  </si>
+  <si>
+    <t>3.25</t>
+  </si>
+  <si>
+    <t>2.85</t>
+  </si>
+  <si>
+    <t>p8KPu8oB</t>
+  </si>
+  <si>
+    <t>SCHOTTLAND League One</t>
+  </si>
+  <si>
+    <t>Montrose</t>
+  </si>
+  <si>
+    <t>Peterhead</t>
+  </si>
+  <si>
+    <t>h4lFkvgg</t>
+  </si>
+  <si>
+    <t>SCHOTTLAND League Two</t>
+  </si>
+  <si>
+    <t>Annan</t>
+  </si>
+  <si>
+    <t>Dumbarton</t>
+  </si>
+  <si>
+    <t>1.80</t>
+  </si>
+  <si>
+    <t>8hvN3CT9</t>
+  </si>
+  <si>
+    <t>Clyde</t>
+  </si>
+  <si>
+    <t>Elgin</t>
+  </si>
+  <si>
+    <t>1.90</t>
+  </si>
+  <si>
+    <t>v7q6aATH</t>
+  </si>
+  <si>
+    <t>SCHOTTLAND Challenge Cup</t>
+  </si>
+  <si>
+    <t>St. Johnstone</t>
+  </si>
+  <si>
+    <t>Ayr</t>
   </si>
   <si>
     <t>1.65</t>
   </si>
   <si>
-    <t>2.00</t>
-  </si>
-  <si>
-    <t>3.80</t>
-  </si>
-  <si>
-    <t>3.30</t>
-  </si>
-  <si>
-    <t>5.00</t>
-  </si>
-  <si>
-    <t>3.70</t>
-  </si>
-  <si>
-    <t>va3kThlL</t>
-  </si>
-  <si>
-    <t>ENGLAND Championship</t>
-  </si>
-  <si>
-    <t>Sheffield United</t>
-  </si>
-  <si>
-    <t>FC Middlesbrough</t>
-  </si>
-  <si>
-    <t>2.20</t>
-  </si>
-  <si>
-    <t>3.40</t>
-  </si>
-  <si>
-    <t>2.75</t>
-  </si>
-  <si>
-    <t>IJmCYLIj</t>
-  </si>
-  <si>
-    <t>SPANIEN La Liga</t>
-  </si>
-  <si>
-    <t>FC Villarreal</t>
-  </si>
-  <si>
-    <t>Espanyol Barcelona</t>
-  </si>
-  <si>
-    <t>1.62</t>
-  </si>
-  <si>
-    <t>1.67</t>
-  </si>
-  <si>
-    <t>4.33</t>
+    <t>dpRRonU1</t>
+  </si>
+  <si>
+    <t>FC Chelsea</t>
+  </si>
+  <si>
+    <t>Leeds United</t>
+  </si>
+  <si>
+    <t>1.60</t>
+  </si>
+  <si>
+    <t>1.53</t>
+  </si>
+  <si>
+    <t>3.90</t>
   </si>
   <si>
     <t>5.25</t>
   </si>
   <si>
-    <t>4.50</t>
-  </si>
-  <si>
-    <t>Euh8YaHb</t>
-  </si>
-  <si>
-    <t>ARGENTINIEN Liga Profesional</t>
-  </si>
-  <si>
-    <t>Barracas Central</t>
-  </si>
-  <si>
-    <t>Gimnasia y Esgrima La Plata</t>
-  </si>
-  <si>
-    <t>2.40</t>
+    <t>5.75</t>
+  </si>
+  <si>
+    <t>rw7M7TjL</t>
+  </si>
+  <si>
+    <t>FC Everton</t>
+  </si>
+  <si>
+    <t>AFC Bournemouth</t>
+  </si>
+  <si>
+    <t>OAseMS5E</t>
+  </si>
+  <si>
+    <t>Tottenham Hotspur</t>
+  </si>
+  <si>
+    <t>Newcastle United</t>
+  </si>
+  <si>
+    <t>2.80</t>
+  </si>
+  <si>
+    <t>2eZ2sKxe</t>
+  </si>
+  <si>
+    <t>SCHWEIZ Super League</t>
+  </si>
+  <si>
+    <t>FC Luzern</t>
+  </si>
+  <si>
+    <t>Grasshoppers Zürich</t>
+  </si>
+  <si>
+    <t>1.91</t>
+  </si>
+  <si>
+    <t>0SATJc97</t>
+  </si>
+  <si>
+    <t>ITALIEN Serie B</t>
+  </si>
+  <si>
+    <t>Calcio Padova</t>
+  </si>
+  <si>
+    <t>Carrarese Calcio</t>
+  </si>
+  <si>
+    <t>2.50</t>
   </si>
   <si>
     <t>2.57</t>
   </si>
   <si>
-    <t>2.85</t>
-  </si>
-  <si>
-    <t>tbje7pP9</t>
-  </si>
-  <si>
-    <t>DÄNEMARK Superliga</t>
-  </si>
-  <si>
-    <t>Aarhus GF</t>
-  </si>
-  <si>
-    <t>Odense BK</t>
-  </si>
-  <si>
-    <t>1.61</t>
-  </si>
-  <si>
-    <t>1.56</t>
-  </si>
-  <si>
-    <t>3.90</t>
-  </si>
-  <si>
-    <t>4.10</t>
-  </si>
-  <si>
-    <t>4.75</t>
-  </si>
-  <si>
-    <t>QRHiwdZQ</t>
-  </si>
-  <si>
-    <t>ITALIEN Serie A</t>
-  </si>
-  <si>
-    <t>AS Rom</t>
-  </si>
-  <si>
-    <t>Cagliari Calcio</t>
-  </si>
-  <si>
-    <t>1.48</t>
-  </si>
-  <si>
-    <t>1.50</t>
-  </si>
-  <si>
-    <t>3.75</t>
-  </si>
-  <si>
-    <t>4.00</t>
-  </si>
-  <si>
-    <t>8.00</t>
-  </si>
-  <si>
-    <t>7.00</t>
-  </si>
-  <si>
-    <t>Esqc7Ijm</t>
-  </si>
-  <si>
-    <t>FRANKREICH Ligue 2</t>
-  </si>
-  <si>
-    <t>SC Amiens</t>
-  </si>
-  <si>
-    <t>Clermont Foot</t>
-  </si>
-  <si>
-    <t>2.55</t>
-  </si>
-  <si>
-    <t>2.50</t>
-  </si>
-  <si>
-    <t>fsWgx3t1</t>
-  </si>
-  <si>
-    <t>SPANIEN La Liga2</t>
-  </si>
-  <si>
-    <t>Racing Santander</t>
-  </si>
-  <si>
-    <t>CD Mirandés</t>
-  </si>
-  <si>
-    <t>1.37</t>
-  </si>
-  <si>
-    <t>1.49</t>
-  </si>
-  <si>
-    <t>5.50</t>
-  </si>
-  <si>
-    <t>2FZzGnNb</t>
-  </si>
-  <si>
-    <t>NIEDERLANDE Eerste Divisie</t>
-  </si>
-  <si>
-    <t>Jong AZ</t>
-  </si>
-  <si>
-    <t>Dordrecht</t>
-  </si>
-  <si>
-    <t>2.05</t>
-  </si>
-  <si>
-    <t>2.45</t>
-  </si>
-  <si>
-    <t>StyRRU3K</t>
-  </si>
-  <si>
-    <t>Jong PSV Eindhoven</t>
-  </si>
-  <si>
-    <t>Oss</t>
-  </si>
-  <si>
-    <t>1.96</t>
-  </si>
-  <si>
-    <t>jmb5zllo</t>
-  </si>
-  <si>
-    <t>FC Famalicão</t>
-  </si>
-  <si>
-    <t>AFS</t>
-  </si>
-  <si>
-    <t>1.35</t>
-  </si>
-  <si>
-    <t>4.20</t>
-  </si>
-  <si>
-    <t>8.50</t>
-  </si>
-  <si>
-    <t>MRSTXzOM</t>
-  </si>
-  <si>
-    <t>ISRAEL Ligat ha&amp;#039;Al</t>
-  </si>
-  <si>
-    <t>Hapoel Be'er Sheva</t>
-  </si>
-  <si>
-    <t>Beitar Jerusalem</t>
-  </si>
-  <si>
-    <t>1.80</t>
-  </si>
-  <si>
-    <t>3.60</t>
-  </si>
-  <si>
-    <t>QTbypQJ0</t>
-  </si>
-  <si>
-    <t>POLEN 1. Liga</t>
-  </si>
-  <si>
-    <t>Chrobry Głogów</t>
-  </si>
-  <si>
-    <t>S. Rzeszow</t>
-  </si>
-  <si>
-    <t>1.95</t>
-  </si>
-  <si>
-    <t>3.25</t>
-  </si>
-  <si>
-    <t>jT9wKN8F</t>
-  </si>
-  <si>
-    <t>Vejle</t>
-  </si>
-  <si>
-    <t>FC Fredericia</t>
+    <t>tOmGs11E</t>
+  </si>
+  <si>
+    <t>Delfino Pescara 1936</t>
+  </si>
+  <si>
+    <t>US Catanzaro</t>
+  </si>
+  <si>
+    <t>2.35</t>
+  </si>
+  <si>
+    <t>0ln4WzgD</t>
+  </si>
+  <si>
+    <t>FC Venedig</t>
+  </si>
+  <si>
+    <t>FC Modena</t>
+  </si>
+  <si>
+    <t>1.79</t>
   </si>
   <si>
     <t>1.71</t>
   </si>
   <si>
-    <t>1.91</t>
-  </si>
-  <si>
-    <t>3.50</t>
-  </si>
-  <si>
-    <t>lEULZdgA</t>
-  </si>
-  <si>
-    <t>Maccabi Tel Aviv</t>
-  </si>
-  <si>
-    <t>Maccabi Bnei Raina</t>
-  </si>
-  <si>
-    <t>1.25</t>
-  </si>
-  <si>
-    <t>1.17</t>
-  </si>
-  <si>
-    <t>6.50</t>
-  </si>
-  <si>
-    <t>10.00</t>
-  </si>
-  <si>
-    <t>13.00</t>
-  </si>
-  <si>
-    <t>vPvHAEbE</t>
-  </si>
-  <si>
-    <t>POLEN Ekstraklasa</t>
-  </si>
-  <si>
-    <t>Piast Gliwice</t>
-  </si>
-  <si>
-    <t>Wisła Płock</t>
-  </si>
-  <si>
-    <t>2.10</t>
-  </si>
-  <si>
-    <t>xQas7BSF</t>
-  </si>
-  <si>
-    <t>PORTUGAL Liga Portugal 2</t>
-  </si>
-  <si>
-    <t>Portimonense SC</t>
-  </si>
-  <si>
-    <t>Benfica Lissabon B</t>
-  </si>
-  <si>
-    <t>2.70</t>
-  </si>
-  <si>
-    <t>SrGvLbMs</t>
-  </si>
-  <si>
-    <t>RUMÄNIEN Superliga</t>
-  </si>
-  <si>
-    <t>Dinamo Bukarest</t>
-  </si>
-  <si>
-    <t>CS Universitatea Craiova</t>
-  </si>
-  <si>
-    <t>2.15</t>
-  </si>
-  <si>
-    <t>EToDHN6j</t>
-  </si>
-  <si>
-    <t>Atalanta Bergamo</t>
-  </si>
-  <si>
-    <t>US Cremonese</t>
-  </si>
-  <si>
-    <t>1.29</t>
-  </si>
-  <si>
-    <t>1.36</t>
-  </si>
-  <si>
-    <t>9.00</t>
-  </si>
-  <si>
-    <t>QeRyfGcU</t>
-  </si>
-  <si>
-    <t>TÜRKEI Süper Lig</t>
-  </si>
-  <si>
-    <t>Fenerbahçe Istanbul</t>
-  </si>
-  <si>
-    <t>Gençlerbirliği</t>
-  </si>
-  <si>
-    <t>1.24</t>
-  </si>
-  <si>
-    <t>1.19</t>
-  </si>
-  <si>
-    <t>6.25</t>
-  </si>
-  <si>
-    <t>9.50</t>
-  </si>
-  <si>
-    <t>x0vooLEa</t>
-  </si>
-  <si>
-    <t>Gaziantep</t>
-  </si>
-  <si>
-    <t>Kasımpaşa Istanbul</t>
-  </si>
-  <si>
-    <t>1.86</t>
-  </si>
-  <si>
-    <t>2.01</t>
-  </si>
-  <si>
-    <t>d2tWLyWQ</t>
-  </si>
-  <si>
-    <t>TÜRKEI 1. Lig</t>
-  </si>
-  <si>
-    <t>Sakaryaspor</t>
-  </si>
-  <si>
-    <t>Erzurumspor</t>
-  </si>
-  <si>
-    <t>1.73</t>
-  </si>
-  <si>
-    <t>GK6oEJrn</t>
-  </si>
-  <si>
-    <t>Kayserispor</t>
-  </si>
-  <si>
-    <t>Kocaelispor</t>
-  </si>
-  <si>
-    <t>2.35</t>
-  </si>
-  <si>
-    <t>U3G1imcT</t>
-  </si>
-  <si>
-    <t>SERBIEN Super Liga</t>
-  </si>
-  <si>
-    <t>OFK Beograd</t>
-  </si>
-  <si>
-    <t>FK Čukarički</t>
-  </si>
-  <si>
-    <t>OIym6Rhl</t>
-  </si>
-  <si>
-    <t>SINGAPUR Premier League</t>
-  </si>
-  <si>
-    <t>Albirex Niigata</t>
-  </si>
-  <si>
-    <t>Hougang</t>
+    <t>lliOuuWQ</t>
+  </si>
+  <si>
+    <t>Reggiana</t>
+  </si>
+  <si>
+    <t>AC Mantova</t>
+  </si>
+  <si>
+    <t>QT2Fwh0t</t>
+  </si>
+  <si>
+    <t>Virtus Entella</t>
+  </si>
+  <si>
+    <t>AC Cesena</t>
+  </si>
+  <si>
+    <t>8YXfzJgl</t>
+  </si>
+  <si>
+    <t>Sampdoria Genua</t>
+  </si>
+  <si>
+    <t>Palermo</t>
   </si>
 </sst>
 </file>
@@ -1533,10 +1470,10 @@
     <col min="1" max="1" width="9.140625" customWidth="1" style="4"/>
     <col min="2" max="2" width="12.1948787144252" customWidth="1" style="4"/>
     <col min="3" max="3" width="13.093129839216" customWidth="1" style="4"/>
-    <col min="4" max="4" width="27.2111554827009" customWidth="1" style="4"/>
+    <col min="4" max="4" width="26.7968139648438" customWidth="1" style="4"/>
     <col min="5" max="5" width="10.5382559640067" customWidth="1" style="6"/>
-    <col min="6" max="6" width="18.5386287144252" customWidth="1" style="4"/>
-    <col min="7" max="7" width="25.0064479282924" customWidth="1" style="4"/>
+    <col min="6" max="6" width="19.1360996791295" customWidth="1" style="4"/>
+    <col min="7" max="7" width="20.7515193394252" customWidth="1" style="4"/>
     <col min="8" max="8" width="9.140625" customWidth="1" style="4"/>
     <col min="9" max="9" width="9.64744567871094" customWidth="1" style="4"/>
     <col min="10" max="10" width="9.140625" customWidth="1" style="4"/>
@@ -2444,7 +2381,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4">
-        <v>64080</v>
+        <v>64093</v>
       </c>
       <c r="B2" s="4" t="b">
         <v>0</v>
@@ -2456,7 +2393,7 @@
         <v>228</v>
       </c>
       <c r="E2" s="6">
-        <v>46062.9895833333</v>
+        <v>46063.96875</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>229</v>
@@ -2474,19 +2411,19 @@
         <v>232</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="9"/>
@@ -2703,25 +2640,25 @@
     </row>
     <row r="3">
       <c r="A3" s="4">
-        <v>64076</v>
+        <v>64109</v>
       </c>
       <c r="B3" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="E3" s="6">
-        <v>46062.9791666667</v>
+        <v>46063.96875</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>231</v>
@@ -2730,22 +2667,22 @@
         <v>231</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="P3" s="8"/>
       <c r="Q3" s="9"/>
@@ -2962,25 +2899,25 @@
     </row>
     <row r="4">
       <c r="A4" s="4">
-        <v>64070</v>
+        <v>64097</v>
       </c>
       <c r="B4" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E4" s="6">
-        <v>46062.9590277778</v>
+        <v>46063.9583333333</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>231</v>
@@ -2989,22 +2926,22 @@
         <v>231</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>232</v>
+        <v>251</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>243</v>
+        <v>253</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>234</v>
+        <v>255</v>
       </c>
       <c r="P4" s="8"/>
       <c r="Q4" s="9"/>
@@ -3221,25 +3158,25 @@
     </row>
     <row r="5">
       <c r="A5" s="4">
-        <v>64066</v>
+        <v>64108</v>
       </c>
       <c r="B5" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="E5" s="6">
-        <v>46062.9583333333</v>
+        <v>46063.9583333333</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>231</v>
@@ -3248,19 +3185,19 @@
         <v>231</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="O5" s="9" t="s">
         <v>261</v>
@@ -3480,25 +3417,25 @@
     </row>
     <row r="6">
       <c r="A6" s="4">
-        <v>64067</v>
+        <v>64110</v>
       </c>
       <c r="B6" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="E6" s="6">
-        <v>46062.9583333333</v>
+        <v>46063.9583333333</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>231</v>
@@ -3507,22 +3444,22 @@
         <v>231</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>235</v>
+        <v>263</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>234</v>
+        <v>270</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="P6" s="8"/>
       <c r="Q6" s="9"/>
@@ -3739,25 +3676,25 @@
     </row>
     <row r="7">
       <c r="A7" s="4">
-        <v>64069</v>
+        <v>64094</v>
       </c>
       <c r="B7" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="E7" s="6">
-        <v>46062.9583333333</v>
+        <v>46063.9479166667</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>231</v>
@@ -3766,22 +3703,22 @@
         <v>231</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="P7" s="8"/>
       <c r="Q7" s="9"/>
@@ -3998,19 +3935,19 @@
     </row>
     <row r="8">
       <c r="A8" s="4">
-        <v>64065</v>
+        <v>64095</v>
       </c>
       <c r="B8" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>279</v>
+        <v>248</v>
       </c>
       <c r="E8" s="6">
-        <v>46062.9479166667</v>
+        <v>46063.9479166667</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>280</v>
@@ -4025,22 +3962,22 @@
         <v>231</v>
       </c>
       <c r="J8" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="K8" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="L8" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="N8" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="L8" s="8" t="s">
+      <c r="O8" s="9" t="s">
         <v>284</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="N8" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="O8" s="9" t="s">
-        <v>287</v>
       </c>
       <c r="P8" s="8"/>
       <c r="Q8" s="9"/>
@@ -4257,25 +4194,25 @@
     </row>
     <row r="9">
       <c r="A9" s="4">
-        <v>64071</v>
+        <v>64096</v>
       </c>
       <c r="B9" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>289</v>
+        <v>248</v>
       </c>
       <c r="E9" s="6">
-        <v>46062.9479166667</v>
+        <v>46063.9479166667</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>231</v>
@@ -4284,22 +4221,22 @@
         <v>231</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>235</v>
+        <v>277</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>234</v>
+        <v>262</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>293</v>
+        <v>246</v>
       </c>
       <c r="P9" s="8"/>
       <c r="Q9" s="9"/>
@@ -4516,25 +4453,25 @@
     </row>
     <row r="10">
       <c r="A10" s="4">
-        <v>64085</v>
+        <v>64098</v>
       </c>
       <c r="B10" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="E10" s="6">
-        <v>46062.9375</v>
+        <v>46063.9479166667</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>231</v>
@@ -4543,22 +4480,22 @@
         <v>231</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>259</v>
+        <v>277</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>300</v>
+        <v>244</v>
       </c>
       <c r="P10" s="8"/>
       <c r="Q10" s="9"/>
@@ -4775,25 +4712,25 @@
     </row>
     <row r="11">
       <c r="A11" s="4">
-        <v>64074</v>
+        <v>64099</v>
       </c>
       <c r="B11" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="E11" s="6">
-        <v>46062.9166666667</v>
+        <v>46063.9479166667</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>231</v>
@@ -4802,22 +4739,22 @@
         <v>231</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>245</v>
+        <v>262</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>268</v>
+        <v>295</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="P11" s="8"/>
       <c r="Q11" s="9"/>
@@ -5034,25 +4971,25 @@
     </row>
     <row r="12">
       <c r="A12" s="4">
-        <v>64075</v>
+        <v>64100</v>
       </c>
       <c r="B12" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>302</v>
       </c>
       <c r="E12" s="6">
-        <v>46062.9166666667</v>
+        <v>46063.9479166667</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>231</v>
@@ -5061,22 +4998,22 @@
         <v>231</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>310</v>
+        <v>277</v>
       </c>
       <c r="K12" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="O12" s="9" t="s">
         <v>305</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="M12" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="N12" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="O12" s="9" t="s">
-        <v>235</v>
       </c>
       <c r="P12" s="8"/>
       <c r="Q12" s="9"/>
@@ -5293,25 +5230,25 @@
     </row>
     <row r="13">
       <c r="A13" s="4">
-        <v>64079</v>
+        <v>64101</v>
       </c>
       <c r="B13" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>228</v>
+        <v>302</v>
       </c>
       <c r="E13" s="6">
-        <v>46062.90625</v>
+        <v>46063.9479166667</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>231</v>
@@ -5320,22 +5257,22 @@
         <v>231</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>286</v>
+        <v>310</v>
       </c>
       <c r="O13" s="9" t="s">
-        <v>316</v>
+        <v>242</v>
       </c>
       <c r="P13" s="8"/>
       <c r="Q13" s="9"/>
@@ -5552,25 +5489,25 @@
     </row>
     <row r="14">
       <c r="A14" s="4">
-        <v>64073</v>
+        <v>64111</v>
       </c>
       <c r="B14" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="E14" s="6">
-        <v>46062.8958333333</v>
+        <v>46063.9479166667</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>231</v>
@@ -5579,22 +5516,22 @@
         <v>231</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>321</v>
+        <v>283</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>321</v>
+        <v>283</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>245</v>
+        <v>269</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>242</v>
+        <v>276</v>
       </c>
       <c r="O14" s="9" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="P14" s="8"/>
       <c r="Q14" s="9"/>
@@ -5811,25 +5748,25 @@
     </row>
     <row r="15">
       <c r="A15" s="4">
-        <v>64078</v>
+        <v>64112</v>
       </c>
       <c r="B15" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="E15" s="6">
-        <v>46062.8958333333</v>
+        <v>46063.9479166667</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>231</v>
@@ -5838,22 +5775,22 @@
         <v>231</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="M15" s="9" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>328</v>
+        <v>263</v>
       </c>
       <c r="P15" s="8"/>
       <c r="Q15" s="9"/>
@@ -6070,25 +6007,25 @@
     </row>
     <row r="16">
       <c r="A16" s="4">
-        <v>64068</v>
+        <v>64113</v>
       </c>
       <c r="B16" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>270</v>
+        <v>316</v>
       </c>
       <c r="E16" s="6">
-        <v>46062.875</v>
+        <v>46063.9479166667</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>231</v>
@@ -6097,22 +6034,22 @@
         <v>231</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>332</v>
+        <v>236</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>334</v>
+        <v>253</v>
       </c>
       <c r="N16" s="8" t="s">
-        <v>285</v>
+        <v>263</v>
       </c>
       <c r="O16" s="9" t="s">
-        <v>245</v>
+        <v>269</v>
       </c>
       <c r="P16" s="8"/>
       <c r="Q16" s="9"/>
@@ -6329,25 +6266,25 @@
     </row>
     <row r="17">
       <c r="A17" s="4">
-        <v>64072</v>
+        <v>64114</v>
       </c>
       <c r="B17" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="E17" s="6">
-        <v>46062.875</v>
+        <v>46063.9479166667</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>231</v>
@@ -6356,22 +6293,22 @@
         <v>231</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>260</v>
+        <v>232</v>
       </c>
       <c r="M17" s="9" t="s">
-        <v>340</v>
+        <v>234</v>
       </c>
       <c r="N17" s="8" t="s">
-        <v>341</v>
+        <v>235</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>342</v>
+        <v>254</v>
       </c>
       <c r="P17" s="8"/>
       <c r="Q17" s="9"/>
@@ -6588,25 +6525,25 @@
     </row>
     <row r="18">
       <c r="A18" s="4">
-        <v>64077</v>
+        <v>64090</v>
       </c>
       <c r="B18" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>344</v>
+        <v>228</v>
       </c>
       <c r="E18" s="6">
-        <v>46062.875</v>
+        <v>46063.9375</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>231</v>
@@ -6615,22 +6552,22 @@
         <v>231</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>305</v>
+        <v>332</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>234</v>
+        <v>334</v>
       </c>
       <c r="M18" s="9" t="s">
-        <v>234</v>
+        <v>255</v>
       </c>
       <c r="N18" s="8" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>251</v>
+        <v>336</v>
       </c>
       <c r="P18" s="8"/>
       <c r="Q18" s="9"/>
@@ -6847,25 +6784,25 @@
     </row>
     <row r="19">
       <c r="A19" s="4">
-        <v>64081</v>
+        <v>64091</v>
       </c>
       <c r="B19" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>349</v>
+        <v>228</v>
       </c>
       <c r="E19" s="6">
-        <v>46062.875</v>
+        <v>46063.9375</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>231</v>
@@ -6874,22 +6811,22 @@
         <v>231</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>292</v>
+        <v>246</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>352</v>
+        <v>300</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="M19" s="9" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="N19" s="8" t="s">
-        <v>306</v>
+        <v>276</v>
       </c>
       <c r="O19" s="9" t="s">
-        <v>232</v>
+        <v>276</v>
       </c>
       <c r="P19" s="8"/>
       <c r="Q19" s="9"/>
@@ -7106,25 +7043,25 @@
     </row>
     <row r="20">
       <c r="A20" s="4">
-        <v>64082</v>
+        <v>64092</v>
       </c>
       <c r="B20" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>354</v>
+        <v>228</v>
       </c>
       <c r="E20" s="6">
-        <v>46062.875</v>
+        <v>46063.9375</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>231</v>
@@ -7133,22 +7070,22 @@
         <v>231</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>306</v>
+        <v>343</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>357</v>
+        <v>262</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
       <c r="M20" s="9" t="s">
-        <v>235</v>
+        <v>269</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>352</v>
+        <v>245</v>
       </c>
       <c r="O20" s="9" t="s">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="P20" s="8"/>
       <c r="Q20" s="9"/>
@@ -7365,25 +7302,25 @@
     </row>
     <row r="21">
       <c r="A21" s="4">
-        <v>64064</v>
+        <v>64115</v>
       </c>
       <c r="B21" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>279</v>
+        <v>345</v>
       </c>
       <c r="E21" s="6">
-        <v>46062.8541666667</v>
+        <v>46063.9375</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>359</v>
+        <v>346</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>231</v>
@@ -7392,22 +7329,22 @@
         <v>231</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>362</v>
+        <v>251</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>244</v>
+        <v>263</v>
       </c>
       <c r="M21" s="9" t="s">
-        <v>244</v>
+        <v>334</v>
       </c>
       <c r="N21" s="8" t="s">
-        <v>341</v>
+        <v>269</v>
       </c>
       <c r="O21" s="9" t="s">
-        <v>363</v>
+        <v>334</v>
       </c>
       <c r="P21" s="8"/>
       <c r="Q21" s="9"/>
@@ -7624,25 +7561,25 @@
     </row>
     <row r="22">
       <c r="A22" s="4">
-        <v>64087</v>
+        <v>64103</v>
       </c>
       <c r="B22" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>364</v>
+        <v>349</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="E22" s="6">
-        <v>46062.8333333333</v>
+        <v>46063.9166666667</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>366</v>
+        <v>351</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>367</v>
+        <v>352</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>231</v>
@@ -7651,22 +7588,22 @@
         <v>231</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>368</v>
+        <v>353</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>369</v>
+        <v>242</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>244</v>
+        <v>262</v>
       </c>
       <c r="M22" s="9" t="s">
-        <v>370</v>
+        <v>288</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>371</v>
+        <v>354</v>
       </c>
       <c r="O22" s="9" t="s">
-        <v>342</v>
+        <v>242</v>
       </c>
       <c r="P22" s="8"/>
       <c r="Q22" s="9"/>
@@ -7883,25 +7820,25 @@
     </row>
     <row r="23">
       <c r="A23" s="4">
-        <v>64088</v>
+        <v>64104</v>
       </c>
       <c r="B23" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>372</v>
+        <v>355</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="E23" s="6">
-        <v>46062.8333333333</v>
+        <v>46063.9166666667</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>373</v>
+        <v>356</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>374</v>
+        <v>357</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>231</v>
@@ -7910,22 +7847,22 @@
         <v>231</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>375</v>
+        <v>295</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>376</v>
+        <v>242</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>334</v>
+        <v>277</v>
       </c>
       <c r="M23" s="9" t="s">
-        <v>251</v>
+        <v>277</v>
       </c>
       <c r="N23" s="8" t="s">
-        <v>245</v>
+        <v>358</v>
       </c>
       <c r="O23" s="9" t="s">
-        <v>334</v>
+        <v>299</v>
       </c>
       <c r="P23" s="8"/>
       <c r="Q23" s="9"/>
@@ -8142,25 +8079,25 @@
     </row>
     <row r="24">
       <c r="A24" s="4">
-        <v>64089</v>
+        <v>64105</v>
       </c>
       <c r="B24" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>377</v>
+        <v>359</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>378</v>
+        <v>350</v>
       </c>
       <c r="E24" s="6">
-        <v>46062.8333333333</v>
+        <v>46063.9166666667</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>379</v>
+        <v>360</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>380</v>
+        <v>361</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>231</v>
@@ -8169,22 +8106,22 @@
         <v>231</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>277</v>
+        <v>362</v>
       </c>
       <c r="K24" s="9" t="s">
-        <v>261</v>
+        <v>363</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>243</v>
+        <v>253</v>
       </c>
       <c r="M24" s="9" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="N24" s="8" t="s">
-        <v>258</v>
+        <v>271</v>
       </c>
       <c r="O24" s="9" t="s">
-        <v>381</v>
+        <v>233</v>
       </c>
       <c r="P24" s="8"/>
       <c r="Q24" s="9"/>
@@ -8401,25 +8338,25 @@
     </row>
     <row r="25">
       <c r="A25" s="4">
-        <v>64086</v>
+        <v>64106</v>
       </c>
       <c r="B25" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>382</v>
+        <v>364</v>
       </c>
       <c r="D25" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="E25" s="6">
+        <v>46063.9166666667</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="E25" s="6">
-        <v>46062.7083333333</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>383</v>
-      </c>
       <c r="G25" s="4" t="s">
-        <v>384</v>
+        <v>366</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>231</v>
@@ -8428,22 +8365,22 @@
         <v>231</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>234</v>
+        <v>358</v>
       </c>
       <c r="K25" s="9" t="s">
-        <v>235</v>
+        <v>358</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>234</v>
+        <v>262</v>
       </c>
       <c r="M25" s="9" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="N25" s="8" t="s">
-        <v>250</v>
+        <v>288</v>
       </c>
       <c r="O25" s="9" t="s">
-        <v>385</v>
+        <v>262</v>
       </c>
       <c r="P25" s="8"/>
       <c r="Q25" s="9"/>
@@ -8660,25 +8597,25 @@
     </row>
     <row r="26">
       <c r="A26" s="4">
-        <v>64083</v>
+        <v>64107</v>
       </c>
       <c r="B26" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>386</v>
+        <v>367</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>387</v>
+        <v>350</v>
       </c>
       <c r="E26" s="6">
-        <v>46062.625</v>
+        <v>46063.9166666667</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>388</v>
+        <v>368</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>389</v>
+        <v>369</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>231</v>
@@ -8687,22 +8624,22 @@
         <v>231</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="K26" s="9" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>334</v>
+        <v>282</v>
       </c>
       <c r="M26" s="9" t="s">
-        <v>334</v>
+        <v>288</v>
       </c>
       <c r="N26" s="8" t="s">
-        <v>292</v>
+        <v>353</v>
       </c>
       <c r="O26" s="9" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="P26" s="8"/>
       <c r="Q26" s="9"/>
@@ -8919,25 +8856,25 @@
     </row>
     <row r="27">
       <c r="A27" s="4">
-        <v>64084</v>
+        <v>64102</v>
       </c>
       <c r="B27" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>391</v>
+        <v>350</v>
       </c>
       <c r="E27" s="6">
-        <v>46062.6041666667</v>
+        <v>46063.875</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>392</v>
+        <v>371</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>393</v>
+        <v>372</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>231</v>
@@ -8946,22 +8883,22 @@
         <v>231</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>283</v>
+        <v>310</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>240</v>
+        <v>269</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>315</v>
+        <v>244</v>
       </c>
       <c r="M27" s="9" t="s">
-        <v>275</v>
+        <v>244</v>
       </c>
       <c r="N27" s="8" t="s">
-        <v>244</v>
+        <v>300</v>
       </c>
       <c r="O27" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="P27" s="8"/>
       <c r="Q27" s="9"/>

</xml_diff>